<commit_message>
graf til problem ferdig
</commit_message>
<xml_diff>
--- a/images/Grafer.xlsx
+++ b/images/Grafer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peran\Documents\Webutvikling\Final project\finalproject\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13D70E3-6A17-4122-AB06-6CB523358C0D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F44092-9B7B-4B53-98A0-A23308F3F6CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{EF2E4AF0-F2A2-4F79-B644-85BB131F6E87}"/>
   </bookViews>
@@ -1189,86 +1189,58 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1356" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1260"/>
-              <a:t>Percentage of people wanting to know how much</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1260" baseline="0"/>
-              <a:t> emissions they produce (out of 315 answers)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB" sz="1260"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1356" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.31968527832247157"/>
+          <c:x val="2.3665368161337932E-2"/>
           <c:y val="0.23307541883175362"/>
-          <c:w val="0.38094430671264101"/>
-          <c:h val="0.56438992284909861"/>
+          <c:w val="0.94976687917913316"/>
+          <c:h val="0.26771037738531978"/>
         </c:manualLayout>
       </c:layout>
-      <c:doughnutChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Agree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="20000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -1295,10 +1267,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1319,10 +1294,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1341,99 +1319,14 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dLbls>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1130" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="50000"/>
-                      <a:lumOff val="50000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Ark1'!$A$6:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Agree</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Don't agree</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Don't know</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$B$6:$B$8</c:f>
+              <c:f>'Ark1'!$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1444,18 +1337,163 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Don't agree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="20000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark1'!$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-135A-4813-A811-71A9BCA507D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Don't know</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="20000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark1'!$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-135A-4813-A811-71A9BCA507D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
+          <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-        <c:holeSize val="50"/>
-      </c:doughnutChart>
+        <c:gapWidth val="100"/>
+        <c:overlap val="100"/>
+        <c:axId val="2021839712"/>
+        <c:axId val="105544640"/>
+      </c:barChart>
+      <c:valAx>
+        <c:axId val="105544640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2021839712"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="2021839712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="105544640"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:solidFill>
           <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1466,42 +1504,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="39000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1130" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -6221,15 +6223,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>747657</xdr:colOff>
+      <xdr:colOff>560820</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>35274</xdr:rowOff>
+      <xdr:rowOff>53591</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>551714</xdr:colOff>
+      <xdr:colOff>364877</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>116812</xdr:rowOff>
+      <xdr:rowOff>135129</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6641,10 +6643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25B0F30-6F18-49B8-B253-71297833591D}">
-  <dimension ref="A2:H8"/>
+  <dimension ref="A2:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6769,6 +6771,20 @@
         <v>40</v>
       </c>
     </row>
+    <row r="24" spans="14:15" x14ac:dyDescent="0.45">
+      <c r="N24">
+        <v>4500</v>
+      </c>
+      <c r="O24">
+        <f>N24*N25</f>
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="25" spans="14:15" x14ac:dyDescent="0.45">
+      <c r="N25">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>